<commit_message>
08.06.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Stock Imei/Mugdho Corporation imei list Main.xlsx
+++ b/2020/Stock Imei/Mugdho Corporation imei list Main.xlsx
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,9 +464,7 @@
       <c r="D2" s="3">
         <v>355569102026809</v>
       </c>
-      <c r="E2" s="3">
-        <v>351918111257661</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3">
         <v>353363111554809</v>
       </c>

</xml_diff>

<commit_message>
10.06.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Stock Imei/Mugdho Corporation imei list Main.xlsx
+++ b/2020/Stock Imei/Mugdho Corporation imei list Main.xlsx
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>